<commit_message>
Update Readme and Carta Gantt
</commit_message>
<xml_diff>
--- a/Carta Gantt.xlsx
+++ b/Carta Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CEDDF2-C573-4A1A-B13B-D3026F619349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0309CC1-C3FB-4836-8E2A-D683216E7212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -159,16 +159,10 @@
     <t>Desarrollo y creación de modelos unimodales</t>
   </si>
   <si>
-    <t>Experimentar/optimizar con diferentes parametros</t>
-  </si>
-  <si>
     <t>Actualización de documentación</t>
   </si>
   <si>
     <t>Aplicación de transformaciones de los datos</t>
-  </si>
-  <si>
-    <t>Analisis de resultados en ambas modalidades</t>
   </si>
   <si>
     <t>Entrenamiento de modelo ensemble facial</t>
@@ -183,40 +177,13 @@
     <t>Análisis y actualización de Papers año 2024 en documentación</t>
   </si>
   <si>
-    <t>Experimentar/optimizar modelo facial con diferentes parametros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Replicación modelos facial de revisiones bibliograficas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Replicación modelos de texto de revisiones bibliograficas </t>
-  </si>
-  <si>
     <t>División y creación de los conjuntos train, validation y test facial</t>
-  </si>
-  <si>
-    <t>División y creación de los conjuntos train, validation y test texto</t>
   </si>
   <si>
     <t>Preparación para la limpieza de datos de texto</t>
   </si>
   <si>
     <t>Creación de data augmentation textual</t>
-  </si>
-  <si>
-    <t>Aplicación de padding y obtención de tokens para modelos pre-entrenados</t>
-  </si>
-  <si>
-    <t>Creación de entrada para modelos pre-entrenados Bert and RoBERTa</t>
-  </si>
-  <si>
-    <t>Creación modelos pre-entrenados textuales</t>
-  </si>
-  <si>
-    <t>Busqueda y optimización de modelos textuales</t>
-  </si>
-  <si>
-    <t>Concadenar datasets textuales</t>
   </si>
   <si>
     <t>Balanceo de datos conjunto de entrenamiento facial</t>
@@ -229,9 +196,6 @@
   </si>
   <si>
     <t>Preprocesamiento de 2 datasets en la modalidad facial</t>
-  </si>
-  <si>
-    <t>Experimentación y ajustes de modelos con 2 datasets</t>
   </si>
   <si>
     <t>Análisis de resultados para 2 datasets facial</t>
@@ -261,13 +225,52 @@
     <t>Resumir documento</t>
   </si>
   <si>
-    <t>Traducir al ingles</t>
-  </si>
-  <si>
     <t>Revisión de documento en español</t>
   </si>
   <si>
-    <t>Revisión de documento en ingles</t>
+    <t>Transferencia a documento de publicación</t>
+  </si>
+  <si>
+    <t>Concatenar datasets textuales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replicación modelos facial de revisiones bibliográficas </t>
+  </si>
+  <si>
+    <t>Experimentar/optimizar modelo facial con diferentes parámetros</t>
+  </si>
+  <si>
+    <t>Experimentar/optimizar con diferentes parámetros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replicación modelos de texto de revisiones bibliográficas </t>
+  </si>
+  <si>
+    <t>Búsqueda y optimización de modelos textuales</t>
+  </si>
+  <si>
+    <t>Análisis de resultados en ambas modalidades</t>
+  </si>
+  <si>
+    <t>Traducir al inglés</t>
+  </si>
+  <si>
+    <t>Revisión de documento en inglés</t>
+  </si>
+  <si>
+    <t>Aplicación de padding y obtención de tokens para modelos preentrenados</t>
+  </si>
+  <si>
+    <t>División y creación de los conjuntos train, validation y test, textuales</t>
+  </si>
+  <si>
+    <t>Creación de entrada para modelos preentrenados Bert y RoBERTa</t>
+  </si>
+  <si>
+    <t>Creación modelos preentrenados textuales</t>
+  </si>
+  <si>
+    <t>Experimentación y ajustes de modelos con 2 datasets (FER2013 + CK+48)</t>
   </si>
 </sst>
 </file>
@@ -1204,19 +1207,10 @@
     <xf numFmtId="166" fontId="23" fillId="44" borderId="2" xfId="10" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="8" applyFont="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="44" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="23" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1225,8 +1219,38 @@
     <xf numFmtId="169" fontId="23" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="43" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="44" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1242,27 +1266,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="44" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="44" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="43" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2122,11 +2125,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:JN53"/>
+  <dimension ref="A1:JN54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="6" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2213,573 +2216,573 @@
         <v>1</v>
       </c>
       <c r="B3" s="43"/>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="58">
+      <c r="D3" s="62"/>
+      <c r="E3" s="65">
         <v>45323</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="I3" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="R3" s="61"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="61"/>
-      <c r="Y3" s="61"/>
-      <c r="Z3" s="61"/>
-      <c r="AA3" s="61"/>
-      <c r="AB3" s="61"/>
-      <c r="AC3" s="61"/>
-      <c r="AD3" s="61"/>
-      <c r="AE3" s="61"/>
-      <c r="AF3" s="61"/>
-      <c r="AG3" s="61"/>
-      <c r="AH3" s="61"/>
-      <c r="AI3" s="61"/>
-      <c r="AJ3" s="61"/>
-      <c r="AK3" s="61"/>
-      <c r="AL3" s="61"/>
-      <c r="AM3" s="61"/>
-      <c r="AN3" s="61"/>
-      <c r="AO3" s="61"/>
-      <c r="AP3" s="61"/>
-      <c r="AQ3" s="61"/>
-      <c r="AR3" s="61"/>
-      <c r="AS3" s="61"/>
-      <c r="AT3" s="61"/>
-      <c r="AU3" s="61"/>
-      <c r="AV3" s="61"/>
-      <c r="AW3" s="61"/>
-      <c r="AX3" s="61"/>
-      <c r="AY3" s="61"/>
-      <c r="AZ3" s="61"/>
-      <c r="BA3" s="61"/>
-      <c r="BB3" s="61"/>
-      <c r="BC3" s="61"/>
-      <c r="BD3" s="61"/>
-      <c r="BE3" s="61"/>
-      <c r="BF3" s="61"/>
-      <c r="BG3" s="61"/>
-      <c r="BH3" s="61"/>
-      <c r="BI3" s="61"/>
-      <c r="BJ3" s="61"/>
-      <c r="BK3" s="61"/>
-      <c r="BL3" s="61"/>
-      <c r="BM3" s="61"/>
-      <c r="BN3" s="61"/>
-      <c r="BO3" s="61"/>
-      <c r="BP3" s="61"/>
-      <c r="BQ3" s="61"/>
-      <c r="BR3" s="61"/>
-      <c r="BS3" s="61"/>
-      <c r="BT3" s="61"/>
-      <c r="BU3" s="61"/>
-      <c r="BV3" s="61"/>
-      <c r="BW3" s="61"/>
-      <c r="BX3" s="61"/>
-      <c r="BY3" s="61"/>
-      <c r="BZ3" s="61"/>
-      <c r="CA3" s="61"/>
-      <c r="CB3" s="61"/>
-      <c r="CC3" s="61"/>
-      <c r="CD3" s="61"/>
-      <c r="CE3" s="61"/>
-      <c r="CF3" s="61"/>
-      <c r="CG3" s="61"/>
-      <c r="CH3" s="61"/>
-      <c r="CI3" s="61"/>
-      <c r="CJ3" s="61"/>
-      <c r="CK3" s="61"/>
-      <c r="CL3" s="61"/>
-      <c r="CM3" s="61"/>
-      <c r="CN3" s="61"/>
-      <c r="CO3" s="61"/>
-      <c r="CP3" s="61"/>
-      <c r="CQ3" s="61"/>
-      <c r="CR3" s="61"/>
-      <c r="CS3" s="61"/>
-      <c r="CT3" s="61"/>
-      <c r="CU3" s="61"/>
-      <c r="CV3" s="61"/>
-      <c r="CW3" s="61"/>
-      <c r="CX3" s="61"/>
-      <c r="CY3" s="61"/>
-      <c r="CZ3" s="61"/>
-      <c r="DA3" s="61"/>
-      <c r="DB3" s="61"/>
-      <c r="DC3" s="61"/>
-      <c r="DD3" s="61"/>
-      <c r="DE3" s="61"/>
-      <c r="DF3" s="61"/>
-      <c r="DG3" s="61"/>
-      <c r="DH3" s="61"/>
-      <c r="DI3" s="61"/>
-      <c r="DJ3" s="61"/>
-      <c r="DK3" s="61"/>
-      <c r="DL3" s="61"/>
-      <c r="DM3" s="61"/>
-      <c r="DN3" s="61"/>
-      <c r="DO3" s="61"/>
-      <c r="DP3" s="61"/>
-      <c r="DQ3" s="61"/>
-      <c r="DR3" s="61"/>
-      <c r="DS3" s="61"/>
-      <c r="DT3" s="61"/>
-      <c r="DU3" s="61"/>
-      <c r="DV3" s="61"/>
-      <c r="DW3" s="61"/>
-      <c r="DX3" s="61"/>
-      <c r="DY3" s="61"/>
-      <c r="DZ3" s="61"/>
-      <c r="EA3" s="61"/>
-      <c r="EB3" s="61"/>
-      <c r="EC3" s="61"/>
-      <c r="ED3" s="61"/>
-      <c r="EE3" s="61"/>
-      <c r="EF3" s="61"/>
-      <c r="EG3" s="61"/>
-      <c r="EH3" s="61"/>
-      <c r="EI3" s="61"/>
-      <c r="EJ3" s="61"/>
-      <c r="EK3" s="61"/>
-      <c r="EL3" s="61"/>
-      <c r="EM3" s="61"/>
-      <c r="EN3" s="61"/>
-      <c r="EO3" s="61"/>
-      <c r="EP3" s="61"/>
-      <c r="EQ3" s="61"/>
-      <c r="ER3" s="61"/>
-      <c r="ES3" s="61"/>
-      <c r="ET3" s="61"/>
-      <c r="EU3" s="61"/>
-      <c r="EV3" s="61"/>
-      <c r="EW3" s="61"/>
-      <c r="EX3" s="61"/>
-      <c r="EY3" s="61"/>
-      <c r="EZ3" s="61"/>
-      <c r="FA3" s="61"/>
-      <c r="FB3" s="61"/>
-      <c r="FC3" s="61"/>
-      <c r="FD3" s="61"/>
-      <c r="FE3" s="61"/>
-      <c r="FF3" s="61"/>
-      <c r="FG3" s="61"/>
-      <c r="FH3" s="61"/>
-      <c r="FI3" s="61"/>
-      <c r="FJ3" s="61"/>
-      <c r="FK3" s="61"/>
-      <c r="FL3" s="61"/>
-      <c r="FM3" s="61"/>
+      <c r="F3" s="65"/>
+      <c r="I3" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
+      <c r="X3" s="68"/>
+      <c r="Y3" s="68"/>
+      <c r="Z3" s="68"/>
+      <c r="AA3" s="68"/>
+      <c r="AB3" s="68"/>
+      <c r="AC3" s="68"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="68"/>
+      <c r="AG3" s="68"/>
+      <c r="AH3" s="68"/>
+      <c r="AI3" s="68"/>
+      <c r="AJ3" s="68"/>
+      <c r="AK3" s="68"/>
+      <c r="AL3" s="68"/>
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
+      <c r="AV3" s="68"/>
+      <c r="AW3" s="68"/>
+      <c r="AX3" s="68"/>
+      <c r="AY3" s="68"/>
+      <c r="AZ3" s="68"/>
+      <c r="BA3" s="68"/>
+      <c r="BB3" s="68"/>
+      <c r="BC3" s="68"/>
+      <c r="BD3" s="68"/>
+      <c r="BE3" s="68"/>
+      <c r="BF3" s="68"/>
+      <c r="BG3" s="68"/>
+      <c r="BH3" s="68"/>
+      <c r="BI3" s="68"/>
+      <c r="BJ3" s="68"/>
+      <c r="BK3" s="68"/>
+      <c r="BL3" s="68"/>
+      <c r="BM3" s="68"/>
+      <c r="BN3" s="68"/>
+      <c r="BO3" s="68"/>
+      <c r="BP3" s="68"/>
+      <c r="BQ3" s="68"/>
+      <c r="BR3" s="68"/>
+      <c r="BS3" s="68"/>
+      <c r="BT3" s="68"/>
+      <c r="BU3" s="68"/>
+      <c r="BV3" s="68"/>
+      <c r="BW3" s="68"/>
+      <c r="BX3" s="68"/>
+      <c r="BY3" s="68"/>
+      <c r="BZ3" s="68"/>
+      <c r="CA3" s="68"/>
+      <c r="CB3" s="68"/>
+      <c r="CC3" s="68"/>
+      <c r="CD3" s="68"/>
+      <c r="CE3" s="68"/>
+      <c r="CF3" s="68"/>
+      <c r="CG3" s="68"/>
+      <c r="CH3" s="68"/>
+      <c r="CI3" s="68"/>
+      <c r="CJ3" s="68"/>
+      <c r="CK3" s="68"/>
+      <c r="CL3" s="68"/>
+      <c r="CM3" s="68"/>
+      <c r="CN3" s="68"/>
+      <c r="CO3" s="68"/>
+      <c r="CP3" s="68"/>
+      <c r="CQ3" s="68"/>
+      <c r="CR3" s="68"/>
+      <c r="CS3" s="68"/>
+      <c r="CT3" s="68"/>
+      <c r="CU3" s="68"/>
+      <c r="CV3" s="68"/>
+      <c r="CW3" s="68"/>
+      <c r="CX3" s="68"/>
+      <c r="CY3" s="68"/>
+      <c r="CZ3" s="68"/>
+      <c r="DA3" s="68"/>
+      <c r="DB3" s="68"/>
+      <c r="DC3" s="68"/>
+      <c r="DD3" s="68"/>
+      <c r="DE3" s="68"/>
+      <c r="DF3" s="68"/>
+      <c r="DG3" s="68"/>
+      <c r="DH3" s="68"/>
+      <c r="DI3" s="68"/>
+      <c r="DJ3" s="68"/>
+      <c r="DK3" s="68"/>
+      <c r="DL3" s="68"/>
+      <c r="DM3" s="68"/>
+      <c r="DN3" s="68"/>
+      <c r="DO3" s="68"/>
+      <c r="DP3" s="68"/>
+      <c r="DQ3" s="68"/>
+      <c r="DR3" s="68"/>
+      <c r="DS3" s="68"/>
+      <c r="DT3" s="68"/>
+      <c r="DU3" s="68"/>
+      <c r="DV3" s="68"/>
+      <c r="DW3" s="68"/>
+      <c r="DX3" s="68"/>
+      <c r="DY3" s="68"/>
+      <c r="DZ3" s="68"/>
+      <c r="EA3" s="68"/>
+      <c r="EB3" s="68"/>
+      <c r="EC3" s="68"/>
+      <c r="ED3" s="68"/>
+      <c r="EE3" s="68"/>
+      <c r="EF3" s="68"/>
+      <c r="EG3" s="68"/>
+      <c r="EH3" s="68"/>
+      <c r="EI3" s="68"/>
+      <c r="EJ3" s="68"/>
+      <c r="EK3" s="68"/>
+      <c r="EL3" s="68"/>
+      <c r="EM3" s="68"/>
+      <c r="EN3" s="68"/>
+      <c r="EO3" s="68"/>
+      <c r="EP3" s="68"/>
+      <c r="EQ3" s="68"/>
+      <c r="ER3" s="68"/>
+      <c r="ES3" s="68"/>
+      <c r="ET3" s="68"/>
+      <c r="EU3" s="68"/>
+      <c r="EV3" s="68"/>
+      <c r="EW3" s="68"/>
+      <c r="EX3" s="68"/>
+      <c r="EY3" s="68"/>
+      <c r="EZ3" s="68"/>
+      <c r="FA3" s="68"/>
+      <c r="FB3" s="68"/>
+      <c r="FC3" s="68"/>
+      <c r="FD3" s="68"/>
+      <c r="FE3" s="68"/>
+      <c r="FF3" s="68"/>
+      <c r="FG3" s="68"/>
+      <c r="FH3" s="68"/>
+      <c r="FI3" s="68"/>
+      <c r="FJ3" s="68"/>
+      <c r="FK3" s="68"/>
+      <c r="FL3" s="68"/>
+      <c r="FM3" s="68"/>
     </row>
     <row r="4" spans="1:274" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="42"/>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="14">
         <v>1</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
-      <c r="I4" s="54">
+      <c r="I4" s="51">
         <f>I5</f>
         <v>45320</v>
       </c>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="54">
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="51">
         <f>P5</f>
         <v>45327</v>
       </c>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
-      <c r="U4" s="55"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="54">
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="66"/>
+      <c r="W4" s="51">
         <f>W5</f>
         <v>45334</v>
       </c>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="55"/>
-      <c r="AB4" s="55"/>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="54">
+      <c r="X4" s="52"/>
+      <c r="Y4" s="52"/>
+      <c r="Z4" s="52"/>
+      <c r="AA4" s="52"/>
+      <c r="AB4" s="52"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="51">
         <f>AD5</f>
         <v>45341</v>
       </c>
-      <c r="AE4" s="55"/>
-      <c r="AF4" s="55"/>
-      <c r="AG4" s="55"/>
-      <c r="AH4" s="55"/>
-      <c r="AI4" s="55"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="54">
+      <c r="AE4" s="52"/>
+      <c r="AF4" s="52"/>
+      <c r="AG4" s="52"/>
+      <c r="AH4" s="52"/>
+      <c r="AI4" s="52"/>
+      <c r="AJ4" s="66"/>
+      <c r="AK4" s="51">
         <f>AK5</f>
         <v>45348</v>
       </c>
-      <c r="AL4" s="55"/>
-      <c r="AM4" s="55"/>
-      <c r="AN4" s="55"/>
-      <c r="AO4" s="55"/>
-      <c r="AP4" s="55"/>
-      <c r="AQ4" s="55"/>
-      <c r="AR4" s="54">
+      <c r="AL4" s="52"/>
+      <c r="AM4" s="52"/>
+      <c r="AN4" s="52"/>
+      <c r="AO4" s="52"/>
+      <c r="AP4" s="52"/>
+      <c r="AQ4" s="52"/>
+      <c r="AR4" s="51">
         <f>AR5</f>
         <v>45355</v>
       </c>
-      <c r="AS4" s="55"/>
-      <c r="AT4" s="55"/>
-      <c r="AU4" s="55"/>
-      <c r="AV4" s="55"/>
-      <c r="AW4" s="55"/>
-      <c r="AX4" s="55"/>
-      <c r="AY4" s="54">
+      <c r="AS4" s="52"/>
+      <c r="AT4" s="52"/>
+      <c r="AU4" s="52"/>
+      <c r="AV4" s="52"/>
+      <c r="AW4" s="52"/>
+      <c r="AX4" s="52"/>
+      <c r="AY4" s="51">
         <f>AY5</f>
         <v>45362</v>
       </c>
-      <c r="AZ4" s="55"/>
-      <c r="BA4" s="55"/>
-      <c r="BB4" s="55"/>
-      <c r="BC4" s="55"/>
-      <c r="BD4" s="55"/>
-      <c r="BE4" s="55"/>
-      <c r="BF4" s="54">
+      <c r="AZ4" s="52"/>
+      <c r="BA4" s="52"/>
+      <c r="BB4" s="52"/>
+      <c r="BC4" s="52"/>
+      <c r="BD4" s="52"/>
+      <c r="BE4" s="52"/>
+      <c r="BF4" s="51">
         <f>BF5</f>
         <v>45369</v>
       </c>
-      <c r="BG4" s="55"/>
-      <c r="BH4" s="55"/>
-      <c r="BI4" s="55"/>
-      <c r="BJ4" s="55"/>
-      <c r="BK4" s="55"/>
-      <c r="BL4" s="55"/>
-      <c r="BM4" s="54">
+      <c r="BG4" s="52"/>
+      <c r="BH4" s="52"/>
+      <c r="BI4" s="52"/>
+      <c r="BJ4" s="52"/>
+      <c r="BK4" s="52"/>
+      <c r="BL4" s="52"/>
+      <c r="BM4" s="51">
         <f>BM5</f>
         <v>45376</v>
       </c>
-      <c r="BN4" s="55"/>
-      <c r="BO4" s="55"/>
-      <c r="BP4" s="55"/>
-      <c r="BQ4" s="55"/>
-      <c r="BR4" s="55"/>
-      <c r="BS4" s="55"/>
-      <c r="BT4" s="54">
+      <c r="BN4" s="52"/>
+      <c r="BO4" s="52"/>
+      <c r="BP4" s="52"/>
+      <c r="BQ4" s="52"/>
+      <c r="BR4" s="52"/>
+      <c r="BS4" s="52"/>
+      <c r="BT4" s="51">
         <f>BT5</f>
         <v>45383</v>
       </c>
-      <c r="BU4" s="55"/>
-      <c r="BV4" s="55"/>
-      <c r="BW4" s="55"/>
-      <c r="BX4" s="55"/>
-      <c r="BY4" s="55"/>
-      <c r="BZ4" s="55"/>
-      <c r="CA4" s="54">
+      <c r="BU4" s="52"/>
+      <c r="BV4" s="52"/>
+      <c r="BW4" s="52"/>
+      <c r="BX4" s="52"/>
+      <c r="BY4" s="52"/>
+      <c r="BZ4" s="52"/>
+      <c r="CA4" s="51">
         <f>CA5</f>
         <v>45390</v>
       </c>
-      <c r="CB4" s="55"/>
-      <c r="CC4" s="55"/>
-      <c r="CD4" s="55"/>
-      <c r="CE4" s="55"/>
-      <c r="CF4" s="55"/>
-      <c r="CG4" s="55"/>
-      <c r="CH4" s="54">
+      <c r="CB4" s="52"/>
+      <c r="CC4" s="52"/>
+      <c r="CD4" s="52"/>
+      <c r="CE4" s="52"/>
+      <c r="CF4" s="52"/>
+      <c r="CG4" s="52"/>
+      <c r="CH4" s="51">
         <f>CH5</f>
         <v>45397</v>
       </c>
-      <c r="CI4" s="55"/>
-      <c r="CJ4" s="55"/>
-      <c r="CK4" s="55"/>
-      <c r="CL4" s="55"/>
-      <c r="CM4" s="55"/>
-      <c r="CN4" s="55"/>
-      <c r="CO4" s="54">
+      <c r="CI4" s="52"/>
+      <c r="CJ4" s="52"/>
+      <c r="CK4" s="52"/>
+      <c r="CL4" s="52"/>
+      <c r="CM4" s="52"/>
+      <c r="CN4" s="52"/>
+      <c r="CO4" s="51">
         <f>CO5</f>
         <v>45404</v>
       </c>
-      <c r="CP4" s="55"/>
-      <c r="CQ4" s="55"/>
-      <c r="CR4" s="55"/>
-      <c r="CS4" s="55"/>
-      <c r="CT4" s="55"/>
-      <c r="CU4" s="55"/>
-      <c r="CV4" s="54">
+      <c r="CP4" s="52"/>
+      <c r="CQ4" s="52"/>
+      <c r="CR4" s="52"/>
+      <c r="CS4" s="52"/>
+      <c r="CT4" s="52"/>
+      <c r="CU4" s="52"/>
+      <c r="CV4" s="51">
         <f>CV5</f>
         <v>45411</v>
       </c>
-      <c r="CW4" s="55"/>
-      <c r="CX4" s="55"/>
-      <c r="CY4" s="55"/>
-      <c r="CZ4" s="55"/>
-      <c r="DA4" s="55"/>
-      <c r="DB4" s="55"/>
-      <c r="DC4" s="54">
+      <c r="CW4" s="52"/>
+      <c r="CX4" s="52"/>
+      <c r="CY4" s="52"/>
+      <c r="CZ4" s="52"/>
+      <c r="DA4" s="52"/>
+      <c r="DB4" s="52"/>
+      <c r="DC4" s="51">
         <f>DC5</f>
         <v>45418</v>
       </c>
-      <c r="DD4" s="55"/>
-      <c r="DE4" s="55"/>
-      <c r="DF4" s="55"/>
-      <c r="DG4" s="55"/>
-      <c r="DH4" s="55"/>
-      <c r="DI4" s="55"/>
-      <c r="DJ4" s="54">
+      <c r="DD4" s="52"/>
+      <c r="DE4" s="52"/>
+      <c r="DF4" s="52"/>
+      <c r="DG4" s="52"/>
+      <c r="DH4" s="52"/>
+      <c r="DI4" s="52"/>
+      <c r="DJ4" s="51">
         <f>DJ5</f>
         <v>45425</v>
       </c>
-      <c r="DK4" s="55"/>
-      <c r="DL4" s="55"/>
-      <c r="DM4" s="55"/>
-      <c r="DN4" s="55"/>
-      <c r="DO4" s="55"/>
-      <c r="DP4" s="55"/>
-      <c r="DQ4" s="54">
+      <c r="DK4" s="52"/>
+      <c r="DL4" s="52"/>
+      <c r="DM4" s="52"/>
+      <c r="DN4" s="52"/>
+      <c r="DO4" s="52"/>
+      <c r="DP4" s="52"/>
+      <c r="DQ4" s="51">
         <f>DQ5</f>
         <v>45432</v>
       </c>
-      <c r="DR4" s="55"/>
-      <c r="DS4" s="55"/>
-      <c r="DT4" s="55"/>
-      <c r="DU4" s="55"/>
-      <c r="DV4" s="55"/>
-      <c r="DW4" s="55"/>
-      <c r="DX4" s="54">
+      <c r="DR4" s="52"/>
+      <c r="DS4" s="52"/>
+      <c r="DT4" s="52"/>
+      <c r="DU4" s="52"/>
+      <c r="DV4" s="52"/>
+      <c r="DW4" s="52"/>
+      <c r="DX4" s="51">
         <f>DX5</f>
         <v>45439</v>
       </c>
-      <c r="DY4" s="55"/>
-      <c r="DZ4" s="55"/>
-      <c r="EA4" s="55"/>
-      <c r="EB4" s="55"/>
-      <c r="EC4" s="55"/>
-      <c r="ED4" s="55"/>
-      <c r="EE4" s="54">
+      <c r="DY4" s="52"/>
+      <c r="DZ4" s="52"/>
+      <c r="EA4" s="52"/>
+      <c r="EB4" s="52"/>
+      <c r="EC4" s="52"/>
+      <c r="ED4" s="52"/>
+      <c r="EE4" s="51">
         <f>EE5</f>
         <v>45446</v>
       </c>
-      <c r="EF4" s="55"/>
-      <c r="EG4" s="55"/>
-      <c r="EH4" s="55"/>
-      <c r="EI4" s="55"/>
-      <c r="EJ4" s="55"/>
-      <c r="EK4" s="55"/>
-      <c r="EL4" s="54">
+      <c r="EF4" s="52"/>
+      <c r="EG4" s="52"/>
+      <c r="EH4" s="52"/>
+      <c r="EI4" s="52"/>
+      <c r="EJ4" s="52"/>
+      <c r="EK4" s="52"/>
+      <c r="EL4" s="51">
         <f>EL5</f>
         <v>45453</v>
       </c>
-      <c r="EM4" s="55"/>
-      <c r="EN4" s="55"/>
-      <c r="EO4" s="55"/>
-      <c r="EP4" s="55"/>
-      <c r="EQ4" s="55"/>
-      <c r="ER4" s="55"/>
-      <c r="ES4" s="54">
+      <c r="EM4" s="52"/>
+      <c r="EN4" s="52"/>
+      <c r="EO4" s="52"/>
+      <c r="EP4" s="52"/>
+      <c r="EQ4" s="52"/>
+      <c r="ER4" s="52"/>
+      <c r="ES4" s="51">
         <f>ES5</f>
         <v>45460</v>
       </c>
-      <c r="ET4" s="55"/>
-      <c r="EU4" s="55"/>
-      <c r="EV4" s="55"/>
-      <c r="EW4" s="55"/>
-      <c r="EX4" s="55"/>
-      <c r="EY4" s="55"/>
-      <c r="EZ4" s="54">
+      <c r="ET4" s="52"/>
+      <c r="EU4" s="52"/>
+      <c r="EV4" s="52"/>
+      <c r="EW4" s="52"/>
+      <c r="EX4" s="52"/>
+      <c r="EY4" s="52"/>
+      <c r="EZ4" s="51">
         <f>EZ5</f>
         <v>45467</v>
       </c>
-      <c r="FA4" s="55"/>
-      <c r="FB4" s="55"/>
-      <c r="FC4" s="55"/>
-      <c r="FD4" s="55"/>
-      <c r="FE4" s="55"/>
-      <c r="FF4" s="55"/>
-      <c r="FG4" s="54">
+      <c r="FA4" s="52"/>
+      <c r="FB4" s="52"/>
+      <c r="FC4" s="52"/>
+      <c r="FD4" s="52"/>
+      <c r="FE4" s="52"/>
+      <c r="FF4" s="52"/>
+      <c r="FG4" s="51">
         <f>FG5</f>
         <v>45474</v>
       </c>
-      <c r="FH4" s="55"/>
-      <c r="FI4" s="55"/>
-      <c r="FJ4" s="55"/>
-      <c r="FK4" s="55"/>
-      <c r="FL4" s="55"/>
-      <c r="FM4" s="55"/>
-      <c r="FN4" s="54">
+      <c r="FH4" s="52"/>
+      <c r="FI4" s="52"/>
+      <c r="FJ4" s="52"/>
+      <c r="FK4" s="52"/>
+      <c r="FL4" s="52"/>
+      <c r="FM4" s="52"/>
+      <c r="FN4" s="51">
         <f>FN5</f>
         <v>45481</v>
       </c>
-      <c r="FO4" s="55"/>
-      <c r="FP4" s="55"/>
-      <c r="FQ4" s="55"/>
-      <c r="FR4" s="55"/>
-      <c r="FS4" s="55"/>
-      <c r="FT4" s="55"/>
-      <c r="FU4" s="54">
+      <c r="FO4" s="52"/>
+      <c r="FP4" s="52"/>
+      <c r="FQ4" s="52"/>
+      <c r="FR4" s="52"/>
+      <c r="FS4" s="52"/>
+      <c r="FT4" s="52"/>
+      <c r="FU4" s="51">
         <f>FU5</f>
         <v>45488</v>
       </c>
-      <c r="FV4" s="55"/>
-      <c r="FW4" s="55"/>
-      <c r="FX4" s="55"/>
-      <c r="FY4" s="55"/>
-      <c r="FZ4" s="55"/>
-      <c r="GA4" s="55"/>
-      <c r="GB4" s="54">
+      <c r="FV4" s="52"/>
+      <c r="FW4" s="52"/>
+      <c r="FX4" s="52"/>
+      <c r="FY4" s="52"/>
+      <c r="FZ4" s="52"/>
+      <c r="GA4" s="52"/>
+      <c r="GB4" s="51">
         <f>GB5</f>
         <v>45495</v>
       </c>
-      <c r="GC4" s="55"/>
-      <c r="GD4" s="55"/>
-      <c r="GE4" s="55"/>
-      <c r="GF4" s="55"/>
-      <c r="GG4" s="55"/>
-      <c r="GH4" s="55"/>
-      <c r="GI4" s="54">
+      <c r="GC4" s="52"/>
+      <c r="GD4" s="52"/>
+      <c r="GE4" s="52"/>
+      <c r="GF4" s="52"/>
+      <c r="GG4" s="52"/>
+      <c r="GH4" s="52"/>
+      <c r="GI4" s="51">
         <f>GI5</f>
         <v>45502</v>
       </c>
-      <c r="GJ4" s="55"/>
-      <c r="GK4" s="55"/>
-      <c r="GL4" s="55"/>
-      <c r="GM4" s="55"/>
-      <c r="GN4" s="55"/>
-      <c r="GO4" s="55"/>
-      <c r="GP4" s="54">
+      <c r="GJ4" s="52"/>
+      <c r="GK4" s="52"/>
+      <c r="GL4" s="52"/>
+      <c r="GM4" s="52"/>
+      <c r="GN4" s="52"/>
+      <c r="GO4" s="52"/>
+      <c r="GP4" s="51">
         <f>GP5</f>
         <v>45509</v>
       </c>
-      <c r="GQ4" s="55"/>
-      <c r="GR4" s="55"/>
-      <c r="GS4" s="55"/>
-      <c r="GT4" s="55"/>
-      <c r="GU4" s="55"/>
-      <c r="GV4" s="55"/>
-      <c r="GW4" s="54">
+      <c r="GQ4" s="52"/>
+      <c r="GR4" s="52"/>
+      <c r="GS4" s="52"/>
+      <c r="GT4" s="52"/>
+      <c r="GU4" s="52"/>
+      <c r="GV4" s="52"/>
+      <c r="GW4" s="51">
         <f>GW5</f>
         <v>45516</v>
       </c>
-      <c r="GX4" s="55"/>
-      <c r="GY4" s="55"/>
-      <c r="GZ4" s="55"/>
-      <c r="HA4" s="55"/>
-      <c r="HB4" s="55"/>
-      <c r="HC4" s="55"/>
-      <c r="HD4" s="54">
+      <c r="GX4" s="52"/>
+      <c r="GY4" s="52"/>
+      <c r="GZ4" s="52"/>
+      <c r="HA4" s="52"/>
+      <c r="HB4" s="52"/>
+      <c r="HC4" s="52"/>
+      <c r="HD4" s="51">
         <f>HD5</f>
         <v>45523</v>
       </c>
-      <c r="HE4" s="55"/>
-      <c r="HF4" s="55"/>
-      <c r="HG4" s="55"/>
-      <c r="HH4" s="55"/>
-      <c r="HI4" s="55"/>
-      <c r="HJ4" s="55"/>
-      <c r="HK4" s="54">
+      <c r="HE4" s="52"/>
+      <c r="HF4" s="52"/>
+      <c r="HG4" s="52"/>
+      <c r="HH4" s="52"/>
+      <c r="HI4" s="52"/>
+      <c r="HJ4" s="52"/>
+      <c r="HK4" s="51">
         <f>HK5</f>
         <v>45530</v>
       </c>
-      <c r="HL4" s="55"/>
-      <c r="HM4" s="55"/>
-      <c r="HN4" s="55"/>
-      <c r="HO4" s="55"/>
-      <c r="HP4" s="55"/>
-      <c r="HQ4" s="55"/>
-      <c r="HR4" s="54">
+      <c r="HL4" s="52"/>
+      <c r="HM4" s="52"/>
+      <c r="HN4" s="52"/>
+      <c r="HO4" s="52"/>
+      <c r="HP4" s="52"/>
+      <c r="HQ4" s="52"/>
+      <c r="HR4" s="51">
         <f>HR5</f>
         <v>45537</v>
       </c>
-      <c r="HS4" s="55"/>
-      <c r="HT4" s="55"/>
-      <c r="HU4" s="55"/>
-      <c r="HV4" s="55"/>
-      <c r="HW4" s="55"/>
-      <c r="HX4" s="55"/>
-      <c r="HY4" s="54">
+      <c r="HS4" s="52"/>
+      <c r="HT4" s="52"/>
+      <c r="HU4" s="52"/>
+      <c r="HV4" s="52"/>
+      <c r="HW4" s="52"/>
+      <c r="HX4" s="52"/>
+      <c r="HY4" s="51">
         <f>HY5</f>
         <v>45544</v>
       </c>
-      <c r="HZ4" s="55"/>
-      <c r="IA4" s="55"/>
-      <c r="IB4" s="55"/>
-      <c r="IC4" s="55"/>
-      <c r="ID4" s="55"/>
-      <c r="IE4" s="55"/>
-      <c r="IF4" s="54">
+      <c r="HZ4" s="52"/>
+      <c r="IA4" s="52"/>
+      <c r="IB4" s="52"/>
+      <c r="IC4" s="52"/>
+      <c r="ID4" s="52"/>
+      <c r="IE4" s="52"/>
+      <c r="IF4" s="51">
         <f>IF5</f>
         <v>45551</v>
       </c>
-      <c r="IG4" s="55"/>
-      <c r="IH4" s="55"/>
-      <c r="II4" s="55"/>
-      <c r="IJ4" s="55"/>
-      <c r="IK4" s="55"/>
-      <c r="IL4" s="55"/>
-      <c r="IM4" s="54">
+      <c r="IG4" s="52"/>
+      <c r="IH4" s="52"/>
+      <c r="II4" s="52"/>
+      <c r="IJ4" s="52"/>
+      <c r="IK4" s="52"/>
+      <c r="IL4" s="52"/>
+      <c r="IM4" s="51">
         <f>IM5</f>
         <v>45558</v>
       </c>
-      <c r="IN4" s="55"/>
-      <c r="IO4" s="55"/>
-      <c r="IP4" s="55"/>
-      <c r="IQ4" s="55"/>
-      <c r="IR4" s="55"/>
-      <c r="IS4" s="55"/>
-      <c r="IT4" s="54">
+      <c r="IN4" s="52"/>
+      <c r="IO4" s="52"/>
+      <c r="IP4" s="52"/>
+      <c r="IQ4" s="52"/>
+      <c r="IR4" s="52"/>
+      <c r="IS4" s="52"/>
+      <c r="IT4" s="51">
         <f>IT5</f>
         <v>45565</v>
       </c>
-      <c r="IU4" s="55"/>
-      <c r="IV4" s="55"/>
-      <c r="IW4" s="55"/>
-      <c r="IX4" s="55"/>
-      <c r="IY4" s="55"/>
-      <c r="IZ4" s="55"/>
-      <c r="JA4" s="54">
+      <c r="IU4" s="52"/>
+      <c r="IV4" s="52"/>
+      <c r="IW4" s="52"/>
+      <c r="IX4" s="52"/>
+      <c r="IY4" s="52"/>
+      <c r="IZ4" s="52"/>
+      <c r="JA4" s="51">
         <f>JA5</f>
         <v>45572</v>
       </c>
-      <c r="JB4" s="55"/>
-      <c r="JC4" s="55"/>
-      <c r="JD4" s="55"/>
-      <c r="JE4" s="55"/>
-      <c r="JF4" s="55"/>
-      <c r="JG4" s="55"/>
-      <c r="JH4" s="54">
+      <c r="JB4" s="52"/>
+      <c r="JC4" s="52"/>
+      <c r="JD4" s="52"/>
+      <c r="JE4" s="52"/>
+      <c r="JF4" s="52"/>
+      <c r="JG4" s="52"/>
+      <c r="JH4" s="51">
         <f>JH5</f>
         <v>45579</v>
       </c>
-      <c r="JI4" s="55"/>
-      <c r="JJ4" s="55"/>
-      <c r="JK4" s="55"/>
-      <c r="JL4" s="55"/>
-      <c r="JM4" s="55"/>
-      <c r="JN4" s="55"/>
+      <c r="JI4" s="52"/>
+      <c r="JJ4" s="52"/>
+      <c r="JK4" s="52"/>
+      <c r="JL4" s="52"/>
+      <c r="JM4" s="52"/>
+      <c r="JN4" s="52"/>
     </row>
     <row r="5" spans="1:274" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
@@ -3861,10 +3864,10 @@
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="67"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="19" t="s">
         <v>8</v>
       </c>
@@ -5228,10 +5231,10 @@
       <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="57"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
       <c r="F8" s="27"/>
@@ -5511,10 +5514,10 @@
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="53"/>
+      <c r="C9" s="58"/>
       <c r="D9" s="29">
         <v>1</v>
       </c>
@@ -5802,10 +5805,10 @@
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="58"/>
       <c r="D10" s="29">
         <v>1</v>
       </c>
@@ -6093,10 +6096,10 @@
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="53"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="29">
         <v>1</v>
       </c>
@@ -6381,10 +6384,10 @@
     </row>
     <row r="12" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="56"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="29">
         <v>1</v>
       </c>
@@ -6668,10 +6671,10 @@
     </row>
     <row r="13" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
-      <c r="B13" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="56"/>
+      <c r="B13" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="60"/>
       <c r="D13" s="29">
         <v>1</v>
       </c>
@@ -6955,10 +6958,10 @@
     </row>
     <row r="14" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
-      <c r="B14" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="56"/>
+      <c r="B14" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="60"/>
       <c r="D14" s="29">
         <v>1</v>
       </c>
@@ -7240,10 +7243,10 @@
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="65"/>
+      <c r="C15" s="55"/>
       <c r="D15" s="32"/>
       <c r="E15" s="33"/>
       <c r="F15" s="34"/>
@@ -7521,10 +7524,10 @@
     </row>
     <row r="16" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="49"/>
+      <c r="C16" s="53"/>
       <c r="D16" s="35">
         <v>1</v>
       </c>
@@ -7808,10 +7811,10 @@
     </row>
     <row r="17" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
-      <c r="B17" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="49"/>
+      <c r="B17" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="53"/>
       <c r="D17" s="35">
         <v>1</v>
       </c>
@@ -8092,10 +8095,10 @@
     </row>
     <row r="18" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
-      <c r="B18" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="49"/>
+      <c r="B18" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="53"/>
       <c r="D18" s="35">
         <v>1</v>
       </c>
@@ -8376,10 +8379,10 @@
     </row>
     <row r="19" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
-      <c r="B19" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="49"/>
+      <c r="B19" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="53"/>
       <c r="D19" s="35">
         <v>1</v>
       </c>
@@ -8663,10 +8666,10 @@
     </row>
     <row r="20" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
-      <c r="B20" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="49"/>
+      <c r="B20" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="53"/>
       <c r="D20" s="35">
         <v>1</v>
       </c>
@@ -8950,10 +8953,10 @@
     </row>
     <row r="21" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
-      <c r="B21" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="49"/>
+      <c r="B21" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="53"/>
       <c r="D21" s="35">
         <v>1</v>
       </c>
@@ -9234,10 +9237,10 @@
     </row>
     <row r="22" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
-      <c r="B22" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="49"/>
+      <c r="B22" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="53"/>
       <c r="D22" s="35">
         <v>1</v>
       </c>
@@ -9518,10 +9521,10 @@
     </row>
     <row r="23" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
-      <c r="B23" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="49"/>
+      <c r="B23" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="53"/>
       <c r="D23" s="35">
         <v>1</v>
       </c>
@@ -9807,10 +9810,10 @@
       <c r="A24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="66"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="37"/>
       <c r="E24" s="38"/>
       <c r="F24" s="39"/>
@@ -10088,10 +10091,10 @@
     </row>
     <row r="25" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
-      <c r="B25" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="50"/>
+      <c r="B25" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="54"/>
       <c r="D25" s="40">
         <v>1</v>
       </c>
@@ -10375,10 +10378,10 @@
     </row>
     <row r="26" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
-      <c r="B26" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="50"/>
+      <c r="B26" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="54"/>
       <c r="D26" s="40">
         <v>1</v>
       </c>
@@ -10659,10 +10662,10 @@
     </row>
     <row r="27" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
-      <c r="B27" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="50"/>
+      <c r="B27" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="54"/>
       <c r="D27" s="40">
         <v>1</v>
       </c>
@@ -10943,10 +10946,10 @@
     </row>
     <row r="28" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
-      <c r="B28" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="50"/>
+      <c r="B28" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="54"/>
       <c r="D28" s="40">
         <v>1</v>
       </c>
@@ -11230,10 +11233,10 @@
     </row>
     <row r="29" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
-      <c r="B29" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="50"/>
+      <c r="B29" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="54"/>
       <c r="D29" s="40">
         <v>1</v>
       </c>
@@ -11517,10 +11520,10 @@
     </row>
     <row r="30" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="50"/>
+      <c r="C30" s="54"/>
       <c r="D30" s="40">
         <v>1</v>
       </c>
@@ -11804,10 +11807,10 @@
     </row>
     <row r="31" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
-      <c r="B31" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="50"/>
+      <c r="B31" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="54"/>
       <c r="D31" s="40">
         <v>1</v>
       </c>
@@ -12091,10 +12094,10 @@
     </row>
     <row r="32" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
-      <c r="B32" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="50"/>
+      <c r="B32" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="54"/>
       <c r="D32" s="40">
         <v>1</v>
       </c>
@@ -12378,10 +12381,10 @@
     </row>
     <row r="33" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
-      <c r="B33" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="50"/>
+      <c r="B33" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="54"/>
       <c r="D33" s="40">
         <v>1</v>
       </c>
@@ -12662,10 +12665,10 @@
     </row>
     <row r="34" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
-      <c r="B34" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="50"/>
+      <c r="B34" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="54"/>
       <c r="D34" s="40">
         <v>1</v>
       </c>
@@ -12946,10 +12949,10 @@
     </row>
     <row r="35" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
-      <c r="B35" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="50"/>
+      <c r="B35" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="54"/>
       <c r="D35" s="40">
         <v>1</v>
       </c>
@@ -13233,10 +13236,10 @@
     </row>
     <row r="36" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
-      <c r="B36" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="50"/>
+      <c r="B36" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="54"/>
       <c r="D36" s="40">
         <v>1</v>
       </c>
@@ -13522,16 +13525,16 @@
       <c r="A37" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="64"/>
+      <c r="B37" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="59"/>
       <c r="D37" s="44"/>
       <c r="E37" s="45"/>
       <c r="F37" s="46"/>
       <c r="G37" s="28"/>
       <c r="H37" s="28" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I37" s="23"/>
       <c r="J37" s="23"/>
@@ -13802,10 +13805,10 @@
     </row>
     <row r="38" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
-      <c r="B38" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="63"/>
+      <c r="B38" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="61"/>
       <c r="D38" s="47">
         <v>1</v>
       </c>
@@ -14086,10 +14089,10 @@
     </row>
     <row r="39" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
-      <c r="B39" s="62" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="62"/>
+      <c r="B39" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="50"/>
       <c r="D39" s="47">
         <v>1</v>
       </c>
@@ -14372,10 +14375,10 @@
     </row>
     <row r="40" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
-      <c r="B40" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="62"/>
+      <c r="B40" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="50"/>
       <c r="D40" s="47">
         <v>1</v>
       </c>
@@ -14656,10 +14659,10 @@
     </row>
     <row r="41" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
-      <c r="B41" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="62"/>
+      <c r="B41" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="50"/>
       <c r="D41" s="47">
         <v>1</v>
       </c>
@@ -14940,10 +14943,10 @@
     </row>
     <row r="42" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
-      <c r="B42" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="62"/>
+      <c r="B42" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="50"/>
       <c r="D42" s="47">
         <v>1</v>
       </c>
@@ -15224,10 +15227,10 @@
     </row>
     <row r="43" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
-      <c r="B43" s="62" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="62"/>
+      <c r="B43" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="50"/>
       <c r="D43" s="47">
         <v>1</v>
       </c>
@@ -15508,10 +15511,10 @@
     </row>
     <row r="44" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
-      <c r="B44" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="62"/>
+      <c r="B44" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="50"/>
       <c r="D44" s="47">
         <v>1</v>
       </c>
@@ -15792,10 +15795,10 @@
     </row>
     <row r="45" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
-      <c r="B45" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="62"/>
+      <c r="B45" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="50"/>
       <c r="D45" s="47">
         <v>1</v>
       </c>
@@ -16078,10 +16081,10 @@
     </row>
     <row r="46" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
-      <c r="B46" s="62" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="62"/>
+      <c r="B46" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="50"/>
       <c r="D46" s="47">
         <v>1</v>
       </c>
@@ -16362,10 +16365,10 @@
     </row>
     <row r="47" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
-      <c r="B47" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" s="62"/>
+      <c r="B47" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="50"/>
       <c r="D47" s="47">
         <v>1</v>
       </c>
@@ -16646,10 +16649,10 @@
     </row>
     <row r="48" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
-      <c r="B48" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" s="62"/>
+      <c r="B48" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="50"/>
       <c r="D48" s="47">
         <v>1</v>
       </c>
@@ -16930,10 +16933,10 @@
     </row>
     <row r="49" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
-      <c r="B49" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="C49" s="62"/>
+      <c r="B49" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="50"/>
       <c r="D49" s="47">
         <v>1</v>
       </c>
@@ -17214,10 +17217,10 @@
     </row>
     <row r="50" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
-      <c r="B50" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="62"/>
+      <c r="B50" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="50"/>
       <c r="D50" s="47">
         <v>1</v>
       </c>
@@ -17498,10 +17501,10 @@
     </row>
     <row r="51" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7"/>
-      <c r="B51" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" s="62"/>
+      <c r="B51" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="50"/>
       <c r="D51" s="47">
         <v>1</v>
       </c>
@@ -17782,23 +17785,21 @@
     </row>
     <row r="52" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
-      <c r="B52" s="62" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" s="62"/>
+      <c r="B52" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="50"/>
       <c r="D52" s="47">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E52" s="48">
         <v>45621</v>
       </c>
       <c r="F52" s="48">
-        <v>45629</v>
+        <v>45642</v>
       </c>
       <c r="G52" s="28"/>
-      <c r="H52" s="28">
-        <v>87</v>
-      </c>
+      <c r="H52" s="28"/>
       <c r="I52" s="23"/>
       <c r="J52" s="23"/>
       <c r="K52" s="23"/>
@@ -18015,42 +18016,42 @@
       <c r="HN52" s="23"/>
       <c r="HO52" s="23"/>
       <c r="HP52" s="23"/>
-      <c r="HQ52" s="23"/>
+      <c r="HQ52" s="24"/>
       <c r="HR52" s="23"/>
       <c r="HS52" s="23"/>
       <c r="HT52" s="23"/>
       <c r="HU52" s="23"/>
       <c r="HV52" s="23"/>
       <c r="HW52" s="23"/>
-      <c r="HX52" s="23"/>
+      <c r="HX52" s="24"/>
       <c r="HY52" s="23"/>
       <c r="HZ52" s="23"/>
       <c r="IA52" s="23"/>
       <c r="IB52" s="23"/>
       <c r="IC52" s="23"/>
       <c r="ID52" s="23"/>
-      <c r="IE52" s="23"/>
+      <c r="IE52" s="24"/>
       <c r="IF52" s="23"/>
       <c r="IG52" s="23"/>
       <c r="IH52" s="23"/>
       <c r="II52" s="23"/>
       <c r="IJ52" s="23"/>
       <c r="IK52" s="23"/>
-      <c r="IL52" s="23"/>
+      <c r="IL52" s="24"/>
       <c r="IM52" s="23"/>
       <c r="IN52" s="23"/>
       <c r="IO52" s="23"/>
       <c r="IP52" s="23"/>
       <c r="IQ52" s="23"/>
       <c r="IR52" s="23"/>
-      <c r="IS52" s="23"/>
+      <c r="IS52" s="24"/>
       <c r="IT52" s="23"/>
       <c r="IU52" s="23"/>
       <c r="IV52" s="23"/>
       <c r="IW52" s="23"/>
       <c r="IX52" s="23"/>
-      <c r="IY52" s="23"/>
-      <c r="IZ52" s="23"/>
+      <c r="IY52" s="24"/>
+      <c r="IZ52" s="24"/>
       <c r="JA52" s="23"/>
       <c r="JB52" s="23"/>
       <c r="JC52" s="23"/>
@@ -18066,34 +18067,350 @@
       <c r="JM52" s="23"/>
       <c r="JN52" s="24"/>
     </row>
-    <row r="53" spans="1:274" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="68"/>
-      <c r="C53" s="68"/>
+    <row r="53" spans="1:274" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7"/>
+      <c r="B53" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="50"/>
+      <c r="D53" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="E53" s="48">
+        <v>45634</v>
+      </c>
+      <c r="F53" s="48">
+        <v>45642</v>
+      </c>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28">
+        <v>87</v>
+      </c>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
+      <c r="K53" s="23"/>
+      <c r="L53" s="23"/>
+      <c r="M53" s="23"/>
+      <c r="N53" s="23"/>
+      <c r="O53" s="23"/>
+      <c r="P53" s="23"/>
+      <c r="Q53" s="23"/>
+      <c r="R53" s="23"/>
+      <c r="S53" s="23"/>
+      <c r="T53" s="23"/>
+      <c r="U53" s="23"/>
+      <c r="V53" s="23"/>
+      <c r="W53" s="23"/>
+      <c r="X53" s="23"/>
+      <c r="Y53" s="23"/>
+      <c r="Z53" s="23"/>
+      <c r="AA53" s="23"/>
+      <c r="AB53" s="23"/>
+      <c r="AC53" s="23"/>
+      <c r="AD53" s="23"/>
+      <c r="AE53" s="23"/>
+      <c r="AF53" s="23"/>
+      <c r="AG53" s="23"/>
+      <c r="AH53" s="23"/>
+      <c r="AI53" s="23"/>
+      <c r="AJ53" s="23"/>
+      <c r="AK53" s="23"/>
+      <c r="AL53" s="23"/>
+      <c r="AM53" s="23"/>
+      <c r="AN53" s="23"/>
+      <c r="AO53" s="23"/>
+      <c r="AP53" s="23"/>
+      <c r="AQ53" s="24"/>
+      <c r="AR53" s="23"/>
+      <c r="AS53" s="23"/>
+      <c r="AT53" s="23"/>
+      <c r="AU53" s="23"/>
+      <c r="AV53" s="23"/>
+      <c r="AW53" s="23"/>
+      <c r="AX53" s="24"/>
+      <c r="AY53" s="23"/>
+      <c r="AZ53" s="23"/>
+      <c r="BA53" s="23"/>
+      <c r="BB53" s="23"/>
+      <c r="BC53" s="23"/>
+      <c r="BD53" s="23"/>
+      <c r="BE53" s="24"/>
+      <c r="BF53" s="23"/>
+      <c r="BG53" s="23"/>
+      <c r="BH53" s="23"/>
+      <c r="BI53" s="23"/>
+      <c r="BJ53" s="23"/>
+      <c r="BK53" s="23"/>
+      <c r="BL53" s="24"/>
+      <c r="BM53" s="23"/>
+      <c r="BN53" s="23"/>
+      <c r="BO53" s="23"/>
+      <c r="BP53" s="23"/>
+      <c r="BQ53" s="23"/>
+      <c r="BR53" s="23"/>
+      <c r="BS53" s="24"/>
+      <c r="BT53" s="23"/>
+      <c r="BU53" s="23"/>
+      <c r="BV53" s="23"/>
+      <c r="BW53" s="23"/>
+      <c r="BX53" s="23"/>
+      <c r="BY53" s="23"/>
+      <c r="BZ53" s="24"/>
+      <c r="CA53" s="23"/>
+      <c r="CB53" s="23"/>
+      <c r="CC53" s="23"/>
+      <c r="CD53" s="23"/>
+      <c r="CE53" s="23"/>
+      <c r="CF53" s="23"/>
+      <c r="CG53" s="24"/>
+      <c r="CH53" s="23"/>
+      <c r="CI53" s="23"/>
+      <c r="CJ53" s="23"/>
+      <c r="CK53" s="23"/>
+      <c r="CL53" s="23"/>
+      <c r="CM53" s="23"/>
+      <c r="CN53" s="24"/>
+      <c r="CO53" s="23"/>
+      <c r="CP53" s="23"/>
+      <c r="CQ53" s="23"/>
+      <c r="CR53" s="23"/>
+      <c r="CS53" s="23"/>
+      <c r="CT53" s="23"/>
+      <c r="CU53" s="24"/>
+      <c r="CV53" s="23"/>
+      <c r="CW53" s="23"/>
+      <c r="CX53" s="23"/>
+      <c r="CY53" s="23"/>
+      <c r="CZ53" s="23"/>
+      <c r="DA53" s="23"/>
+      <c r="DB53" s="24"/>
+      <c r="DC53" s="23"/>
+      <c r="DD53" s="23"/>
+      <c r="DE53" s="23"/>
+      <c r="DF53" s="23"/>
+      <c r="DG53" s="23"/>
+      <c r="DH53" s="23"/>
+      <c r="DI53" s="24"/>
+      <c r="DJ53" s="23"/>
+      <c r="DK53" s="23"/>
+      <c r="DL53" s="23"/>
+      <c r="DM53" s="23"/>
+      <c r="DN53" s="23"/>
+      <c r="DO53" s="23"/>
+      <c r="DP53" s="24"/>
+      <c r="DQ53" s="23"/>
+      <c r="DR53" s="23"/>
+      <c r="DS53" s="23"/>
+      <c r="DT53" s="23"/>
+      <c r="DU53" s="23"/>
+      <c r="DV53" s="23"/>
+      <c r="DW53" s="24"/>
+      <c r="DX53" s="23"/>
+      <c r="DY53" s="23"/>
+      <c r="DZ53" s="23"/>
+      <c r="EA53" s="23"/>
+      <c r="EB53" s="23"/>
+      <c r="EC53" s="23"/>
+      <c r="ED53" s="24"/>
+      <c r="EE53" s="23"/>
+      <c r="EF53" s="23"/>
+      <c r="EG53" s="23"/>
+      <c r="EH53" s="23"/>
+      <c r="EI53" s="23"/>
+      <c r="EJ53" s="23"/>
+      <c r="EK53" s="24"/>
+      <c r="EL53" s="23"/>
+      <c r="EM53" s="23"/>
+      <c r="EN53" s="23"/>
+      <c r="EO53" s="23"/>
+      <c r="EP53" s="23"/>
+      <c r="EQ53" s="23"/>
+      <c r="ER53" s="24"/>
+      <c r="ES53" s="23"/>
+      <c r="ET53" s="23"/>
+      <c r="EU53" s="23"/>
+      <c r="EV53" s="23"/>
+      <c r="EW53" s="23"/>
+      <c r="EX53" s="23"/>
+      <c r="EY53" s="24"/>
+      <c r="EZ53" s="23"/>
+      <c r="FA53" s="23"/>
+      <c r="FB53" s="23"/>
+      <c r="FC53" s="23"/>
+      <c r="FD53" s="23"/>
+      <c r="FE53" s="23"/>
+      <c r="FF53" s="24"/>
+      <c r="FG53" s="23"/>
+      <c r="FH53" s="23"/>
+      <c r="FI53" s="23"/>
+      <c r="FJ53" s="23"/>
+      <c r="FK53" s="23"/>
+      <c r="FL53" s="23"/>
+      <c r="FM53" s="24"/>
+      <c r="FN53" s="23"/>
+      <c r="FO53" s="23"/>
+      <c r="FP53" s="23"/>
+      <c r="FQ53" s="23"/>
+      <c r="FR53" s="23"/>
+      <c r="FS53" s="23"/>
+      <c r="FT53" s="24"/>
+      <c r="FU53" s="23"/>
+      <c r="FV53" s="23"/>
+      <c r="FW53" s="23"/>
+      <c r="FX53" s="23"/>
+      <c r="FY53" s="23"/>
+      <c r="FZ53" s="23"/>
+      <c r="GA53" s="24"/>
+      <c r="GB53" s="23"/>
+      <c r="GC53" s="23"/>
+      <c r="GD53" s="23"/>
+      <c r="GE53" s="23"/>
+      <c r="GF53" s="23"/>
+      <c r="GG53" s="23"/>
+      <c r="GH53" s="24"/>
+      <c r="GI53" s="23"/>
+      <c r="GJ53" s="23"/>
+      <c r="GK53" s="23"/>
+      <c r="GL53" s="23"/>
+      <c r="GM53" s="23"/>
+      <c r="GN53" s="23"/>
+      <c r="GO53" s="24"/>
+      <c r="GP53" s="23"/>
+      <c r="GQ53" s="23"/>
+      <c r="GR53" s="23"/>
+      <c r="GS53" s="23"/>
+      <c r="GT53" s="23"/>
+      <c r="GU53" s="23"/>
+      <c r="GV53" s="24"/>
+      <c r="GW53" s="23"/>
+      <c r="GX53" s="23"/>
+      <c r="GY53" s="23"/>
+      <c r="GZ53" s="23"/>
+      <c r="HA53" s="23"/>
+      <c r="HB53" s="23"/>
+      <c r="HC53" s="24"/>
+      <c r="HD53" s="23"/>
+      <c r="HE53" s="23"/>
+      <c r="HF53" s="23"/>
+      <c r="HG53" s="23"/>
+      <c r="HH53" s="23"/>
+      <c r="HI53" s="23"/>
+      <c r="HJ53" s="24"/>
+      <c r="HK53" s="23"/>
+      <c r="HL53" s="23"/>
+      <c r="HM53" s="23"/>
+      <c r="HN53" s="23"/>
+      <c r="HO53" s="23"/>
+      <c r="HP53" s="23"/>
+      <c r="HQ53" s="23"/>
+      <c r="HR53" s="23"/>
+      <c r="HS53" s="23"/>
+      <c r="HT53" s="23"/>
+      <c r="HU53" s="23"/>
+      <c r="HV53" s="23"/>
+      <c r="HW53" s="23"/>
+      <c r="HX53" s="23"/>
+      <c r="HY53" s="23"/>
+      <c r="HZ53" s="23"/>
+      <c r="IA53" s="23"/>
+      <c r="IB53" s="23"/>
+      <c r="IC53" s="23"/>
+      <c r="ID53" s="23"/>
+      <c r="IE53" s="23"/>
+      <c r="IF53" s="23"/>
+      <c r="IG53" s="23"/>
+      <c r="IH53" s="23"/>
+      <c r="II53" s="23"/>
+      <c r="IJ53" s="23"/>
+      <c r="IK53" s="23"/>
+      <c r="IL53" s="23"/>
+      <c r="IM53" s="23"/>
+      <c r="IN53" s="23"/>
+      <c r="IO53" s="23"/>
+      <c r="IP53" s="23"/>
+      <c r="IQ53" s="23"/>
+      <c r="IR53" s="23"/>
+      <c r="IS53" s="23"/>
+      <c r="IT53" s="23"/>
+      <c r="IU53" s="23"/>
+      <c r="IV53" s="23"/>
+      <c r="IW53" s="23"/>
+      <c r="IX53" s="23"/>
+      <c r="IY53" s="23"/>
+      <c r="IZ53" s="23"/>
+      <c r="JA53" s="23"/>
+      <c r="JB53" s="23"/>
+      <c r="JC53" s="23"/>
+      <c r="JD53" s="23"/>
+      <c r="JE53" s="23"/>
+      <c r="JF53" s="23"/>
+      <c r="JG53" s="24"/>
+      <c r="JH53" s="23"/>
+      <c r="JI53" s="23"/>
+      <c r="JJ53" s="23"/>
+      <c r="JK53" s="23"/>
+      <c r="JL53" s="23"/>
+      <c r="JM53" s="23"/>
+      <c r="JN53" s="24"/>
+    </row>
+    <row r="54" spans="1:274" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="89">
+  <mergeCells count="90">
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="I3:FM3"/>
+    <mergeCell ref="FG4:FM4"/>
     <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="HR4:HX4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="GP4:GV4"/>
-    <mergeCell ref="GW4:HC4"/>
-    <mergeCell ref="HD4:HJ4"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="IT4:IZ4"/>
-    <mergeCell ref="JA4:JG4"/>
-    <mergeCell ref="JH4:JN4"/>
-    <mergeCell ref="HY4:IE4"/>
-    <mergeCell ref="IF4:IL4"/>
-    <mergeCell ref="IM4:IS4"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="FU4:GA4"/>
+    <mergeCell ref="GB4:GH4"/>
+    <mergeCell ref="GI4:GO4"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="FN4:FT4"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="EE4:EK4"/>
+    <mergeCell ref="EL4:ER4"/>
+    <mergeCell ref="ES4:EY4"/>
+    <mergeCell ref="EZ4:FF4"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B33:C33"/>
     <mergeCell ref="HK4:HQ4"/>
     <mergeCell ref="CO4:CU4"/>
     <mergeCell ref="B28:C28"/>
@@ -18110,59 +18427,30 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="FU4:GA4"/>
-    <mergeCell ref="GB4:GH4"/>
-    <mergeCell ref="GI4:GO4"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="FN4:FT4"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="EE4:EK4"/>
-    <mergeCell ref="EL4:ER4"/>
-    <mergeCell ref="ES4:EY4"/>
-    <mergeCell ref="EZ4:FF4"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="I3:FM3"/>
-    <mergeCell ref="FG4:FM4"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="IT4:IZ4"/>
+    <mergeCell ref="JA4:JG4"/>
+    <mergeCell ref="JH4:JN4"/>
+    <mergeCell ref="HY4:IE4"/>
+    <mergeCell ref="IF4:IL4"/>
+    <mergeCell ref="IM4:IS4"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="HR4:HX4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="GP4:GV4"/>
+    <mergeCell ref="GW4:HC4"/>
+    <mergeCell ref="HD4:HJ4"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D52">
+  <conditionalFormatting sqref="D7:D53">
     <cfRule type="dataBar" priority="471">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18176,22 +18464,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:HJ51 HR7:IS51 JA7:JN51 I52:HK52 IP52:JN52 IT7:IZ45">
+  <conditionalFormatting sqref="I7:HJ52 HR7:IS52 JA7:JN52 I53:HK53 IP53:JN53 IT7:IZ45">
     <cfRule type="expression" dxfId="31" priority="236">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HD5:HI51 HR5:HW51 HY5:ID51 IF5:IK51 IM5:IR51 IT5:IY51 JH5:JM51 I5:DO52 DQ5:DV52 DX5:EC52 EE5:EJ52 EL5:EQ52 ES5:EX52 EZ5:FE52 FG5:FL52 FN5:FS52 FU5:FZ52 GB5:GG52 GI5:GN52 GP5:GU52 GW5:HB52 JA5:JF52">
+  <conditionalFormatting sqref="HD5:HI52 HR5:HW52 HY5:ID52 IF5:IK52 IM5:IR52 IT5:IY52 JH5:JM52 I5:DO53 DQ5:DV53 DX5:EC53 EE5:EJ53 EL5:EQ53 ES5:EX53 EZ5:FE53 FG5:FL53 FN5:FS53 FU5:FZ53 GB5:GG53 GI5:GN53 GP5:GU53 GW5:HB53 JA5:JF53">
     <cfRule type="expression" dxfId="30" priority="238">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HD7:HI51 HR7:HW51 HY7:ID51 IF7:IK51 IM7:IR51 IT7:IY51 JH7:JM51 I7:DO52 DQ7:DV52 DX7:EC52 EE7:EJ52 EL7:EQ52 ES7:EX52 EZ7:FE52 FG7:FL52 FN7:FS52 FU7:FZ52 GB7:GG52 GI7:GN52 GP7:GU52 GW7:HB52 JA7:JF52">
+  <conditionalFormatting sqref="HD7:HI52 HR7:HW52 HY7:ID52 IF7:IK52 IM7:IR52 IT7:IY52 JH7:JM52 I7:DO53 DQ7:DV53 DX7:EC53 EE7:EJ53 EL7:EQ53 ES7:EX53 EZ7:FE53 FG7:FL53 FN7:FS53 FU7:FZ53 GB7:GG53 GI7:GN53 GP7:GU53 GW7:HB53 JA7:JF53">
     <cfRule type="expression" dxfId="29" priority="237" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HD52:HI52">
+  <conditionalFormatting sqref="HD53:HI53">
     <cfRule type="expression" dxfId="28" priority="176" stopIfTrue="1">
       <formula>AND(task_end&gt;=HD$5,task_start&lt;HE$5)</formula>
     </cfRule>
@@ -18209,7 +18497,7 @@
       <formula>AND(task_end&gt;=HK$5,task_start&lt;HL$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HK15:HP51">
+  <conditionalFormatting sqref="HK15:HP52">
     <cfRule type="expression" dxfId="24" priority="169" stopIfTrue="1">
       <formula>AND(task_end&gt;=HK$5,task_start&lt;HL$5)</formula>
     </cfRule>
@@ -18222,12 +18510,12 @@
       <formula>AND(task_start&lt;=HK$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=HK$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HK15:HQ51">
+  <conditionalFormatting sqref="HK15:HQ52">
     <cfRule type="expression" dxfId="21" priority="168">
       <formula>AND(task_start&lt;=HK$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=HK$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HK52:IZ52">
+  <conditionalFormatting sqref="HK53:IZ53">
     <cfRule type="expression" dxfId="20" priority="2" stopIfTrue="1">
       <formula>AND(task_end&gt;=HK$5,task_start&lt;HL$5)</formula>
     </cfRule>
@@ -18246,37 +18534,37 @@
       <formula>AND(task_start&lt;=HK$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=HK$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HL52:IO52">
+  <conditionalFormatting sqref="HL53:IO53">
     <cfRule type="expression" dxfId="15" priority="1">
       <formula>AND(task_start&lt;=HL$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=HL$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HQ5:HQ51 HX5:HX51 DP5:DP52 DW5:DW52 ED5:ED52 EK5:EK52 ER5:ER52 EY5:EY52 FF5:FF52 JG5:JG52">
+  <conditionalFormatting sqref="HQ5:HQ52 HX5:HX52 DP5:DP53 DW5:DW53 ED5:ED53 EK5:EK53 ER5:ER53 EY5:EY53 FF5:FF53 JG5:JG53">
     <cfRule type="expression" dxfId="14" priority="492">
       <formula>AND(TODAY()&gt;=DP$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="HQ7:HQ51 HX7:HX51 DP7:DP52 DW7:DW52 ED7:ED52 EK7:EK52 ER7:ER52 EY7:EY52 FF7:FF52 JG7:JG52">
+  <conditionalFormatting sqref="HQ7:HQ52 HX7:HX52 DP7:DP53 DW7:DW53 ED7:ED53 EK7:EK53 ER7:ER53 EY7:EY53 FF7:FF53 JG7:JG53">
     <cfRule type="expression" dxfId="13" priority="496" stopIfTrue="1">
       <formula>AND(task_end&gt;=DP$5,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IE7:IE51 IL7:IL51 GA7:GA52 GH7:GH52 GO7:GO52 GV7:GV52 HC7:HC52 IS7:IS52 HJ7:HJ52 JN7:JN52">
+  <conditionalFormatting sqref="IE7:IE52 IL7:IL52 GA7:GA53 GH7:GH53 GO7:GO53 GV7:GV53 HC7:HC53 IS7:IS53 HJ7:HJ53 JN7:JN53">
     <cfRule type="expression" dxfId="12" priority="233" stopIfTrue="1">
       <formula>AND(task_end&gt;=GA$5,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IS5:IS52 IE5:IE51 IL5:IL51 GA5:GA52 GH5:GH52 GO5:GO52 GV5:GV52 HC5:HC52">
+  <conditionalFormatting sqref="IS5:IS53 IE5:IE52 IL5:IL52 GA5:GA53 GH5:GH53 GO5:GO53 GV5:GV53 HC5:HC53">
     <cfRule type="expression" dxfId="11" priority="232">
       <formula>AND(TODAY()&gt;=GA$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IT46:IX51">
+  <conditionalFormatting sqref="IT46:IX52">
     <cfRule type="expression" dxfId="10" priority="178">
       <formula>AND(task_start&lt;=IT$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=IT$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IY46:IZ51">
+  <conditionalFormatting sqref="IY46:IZ52">
     <cfRule type="expression" dxfId="9" priority="504">
       <formula>AND(task_start&lt;=IZ$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=IZ$5)</formula>
     </cfRule>
@@ -18287,12 +18575,12 @@
       <formula>AND(task_end&gt;=IZ$5,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IZ5:IZ45 FM5:FM52 FT5:FT52 HJ5:HJ52 JN5:JN52">
+  <conditionalFormatting sqref="IZ5:IZ45 FM5:FM53 FT5:FT53 HJ5:HJ53 JN5:JN53">
     <cfRule type="expression" dxfId="6" priority="182">
       <formula>AND(TODAY()&gt;=FM$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IZ46:IZ51">
+  <conditionalFormatting sqref="IZ46:IZ52">
     <cfRule type="expression" dxfId="5" priority="103" stopIfTrue="1">
       <formula>AND(task_end&gt;=IZ$5,task_start&lt;JA$5)</formula>
     </cfRule>
@@ -18300,17 +18588,17 @@
       <formula>AND(TODAY()&gt;=IZ$5,TODAY()&lt;JA$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IZ52 IZ7:IZ45 FM7:FM52 FT7:FT52">
+  <conditionalFormatting sqref="IZ53 IZ7:IZ45 FM7:FM53 FT7:FT53">
     <cfRule type="expression" dxfId="3" priority="260" stopIfTrue="1">
       <formula>AND(task_end&gt;=FM$5,task_start&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="IZ52">
+  <conditionalFormatting sqref="IZ53">
     <cfRule type="expression" dxfId="2" priority="259">
       <formula>AND(TODAY()&gt;=IZ$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="JH52:JM52">
+  <conditionalFormatting sqref="JH53:JM53">
     <cfRule type="expression" dxfId="1" priority="105" stopIfTrue="1">
       <formula>AND(task_end&gt;=JH$5,task_start&lt;JI$5)</formula>
     </cfRule>
@@ -18345,7 +18633,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D52</xm:sqref>
+          <xm:sqref>D7:D53</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -18363,26 +18651,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -18670,6 +18938,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
   <ds:schemaRefs>
@@ -18679,18 +18967,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18709,4 +18985,16 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>